<commit_message>
created t testing tables
</commit_message>
<xml_diff>
--- a/master demographics log.xlsx
+++ b/master demographics log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elisabeth/Desktop/UMASS/BKonline data/BK-Online-Replication/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F3F545-503B-E549-BB86-D5DBB781915E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9370A6-1FD8-4D4B-AFC8-76B5881287AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="500" windowWidth="26120" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4294" uniqueCount="766">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4298" uniqueCount="766">
   <si>
     <t>Experimenter</t>
   </si>
@@ -2896,9 +2896,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y312"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A247" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L264" sqref="L264"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A234" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E253" sqref="E253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17477,6 +17477,12 @@
       <c r="F260">
         <v>5</v>
       </c>
+      <c r="H260" t="s">
+        <v>340</v>
+      </c>
+      <c r="I260" t="s">
+        <v>433</v>
+      </c>
       <c r="J260" t="s">
         <v>374</v>
       </c>
@@ -17546,6 +17552,12 @@
       </c>
       <c r="F262">
         <v>5</v>
+      </c>
+      <c r="H262" t="s">
+        <v>340</v>
+      </c>
+      <c r="I262" t="s">
+        <v>433</v>
       </c>
       <c r="J262" t="s">
         <v>374</v>

</xml_diff>